<commit_message>
fixed error in xy axis labels
</commit_message>
<xml_diff>
--- a/doc/data/export_fitparameters.xlsx
+++ b/doc/data/export_fitparameters.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>3</v>
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -556,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -605,313 +605,235 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.9472680583112575</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2.223919256018393</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>153.7783652645406</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.006025991901023649</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.03184829394997488</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.4129295751577916</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.5298482565860553</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2.244143484104387</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>151.1248275859587</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.003813524678055624</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.03786337253289194</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.3493684817290318</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.2703646303441631</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1.884655015831774</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>152.606459888769</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.01125808542460546</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.1174256480359388</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.5183685442380734</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9472680583112575</v>
+        <v>2.675261005030712e-06</v>
       </c>
       <c r="D13" t="n">
-        <v>2.223919256018393</v>
+        <v>0.115141225199289</v>
       </c>
       <c r="E13" t="n">
-        <v>153.7783652645406</v>
+        <v>196.6459284968385</v>
       </c>
       <c r="F13" t="n">
-        <v>0.006025991901023649</v>
+        <v>4.112191952052441e-06</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03184829394997488</v>
+        <v>0.04134023766356392</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4129295751577916</v>
+        <v>19.0485333989567</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5298482565860553</v>
+        <v>0.09230205106663794</v>
       </c>
       <c r="D14" t="n">
-        <v>2.244143484104387</v>
+        <v>4.669976716007622</v>
       </c>
       <c r="E14" t="n">
-        <v>151.1248275859587</v>
+        <v>127.7166921490056</v>
       </c>
       <c r="F14" t="n">
-        <v>0.003813524678055624</v>
+        <v>0.002932232162550305</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03786337253289194</v>
+        <v>0.5646676157015504</v>
       </c>
       <c r="H14" t="n">
-        <v>0.3493684817290318</v>
+        <v>1.17145605939585</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2703646303441631</v>
+        <v>0.09525889716251723</v>
       </c>
       <c r="D15" t="n">
-        <v>1.884655015831774</v>
+        <v>4.52673159588073</v>
       </c>
       <c r="E15" t="n">
-        <v>152.606459888769</v>
+        <v>127.906352490902</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01125808542460546</v>
+        <v>0.002588878247092757</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1174256480359388</v>
+        <v>0.4959606993867441</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5183685442380734</v>
+        <v>1.237087471771242</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>2.675261005030712e-06</v>
+        <v>0.0344672474065517</v>
       </c>
       <c r="D16" t="n">
-        <v>0.115141225199289</v>
+        <v>2.421714012215387</v>
       </c>
       <c r="E16" t="n">
-        <v>196.6459284968385</v>
+        <v>135.2320396672094</v>
       </c>
       <c r="F16" t="n">
-        <v>4.112191952052441e-06</v>
+        <v>0.001512072145519961</v>
       </c>
       <c r="G16" t="n">
-        <v>0.04134023766356392</v>
+        <v>0.2827222181124596</v>
       </c>
       <c r="H16" t="n">
-        <v>19.0485333989567</v>
+        <v>1.332360855903706</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.09230205106663794</v>
+        <v>0.1098812605152593</v>
       </c>
       <c r="D17" t="n">
-        <v>4.669976716007622</v>
+        <v>2.363978253375465</v>
       </c>
       <c r="E17" t="n">
-        <v>127.7166921490056</v>
+        <v>306.7576531483032</v>
       </c>
       <c r="F17" t="n">
-        <v>0.002932232162550305</v>
+        <v>0.03338903291495714</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5646676157015504</v>
+        <v>1.625401203518225</v>
       </c>
       <c r="H17" t="n">
-        <v>1.17145605939585</v>
+        <v>56.54168194141118</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B18" t="n">
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0.09525889716251723</v>
+        <v>0.09451542193317325</v>
       </c>
       <c r="D18" t="n">
-        <v>4.52673159588073</v>
+        <v>1.402870295725338</v>
       </c>
       <c r="E18" t="n">
-        <v>127.906352490902</v>
+        <v>313.6412579251271</v>
       </c>
       <c r="F18" t="n">
-        <v>0.002588878247092757</v>
+        <v>0.00962626803275661</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4959606993867441</v>
+        <v>0.2332875770487738</v>
       </c>
       <c r="H18" t="n">
-        <v>1.237087471771242</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>27</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0344672474065517</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2.421714012215387</v>
-      </c>
-      <c r="E19" t="n">
-        <v>135.2320396672094</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.001512072145519961</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.2827222181124596</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1.332360855903706</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>31</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.1098812605152593</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2.363978253375465</v>
-      </c>
-      <c r="E20" t="n">
-        <v>306.7576531483032</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.03338903291495714</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1.625401203518225</v>
-      </c>
-      <c r="H20" t="n">
-        <v>56.54168194141118</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>31</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.09451542193317325</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.402870295725338</v>
-      </c>
-      <c r="E21" t="n">
-        <v>313.6412579251271</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.00962626803275661</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.2332875770487738</v>
-      </c>
-      <c r="H21" t="n">
         <v>14.5655640723558</v>
       </c>
     </row>

</xml_diff>